<commit_message>
Fixes up to RCRs and changes to optimization
</commit_message>
<xml_diff>
--- a/data/data.xlsx
+++ b/data/data.xlsx
@@ -177,7 +177,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" mc:Ignorable="x14ac">
   <numFmts count="0"/>
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -195,12 +195,6 @@
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
     </font>
@@ -232,7 +226,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="7">
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0"/>
     <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -244,9 +238,6 @@
       <alignment horizontal="general"/>
     </xf>
     <xf xfId="0" numFmtId="4" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf xfId="0" numFmtId="4" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="3" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
@@ -563,19 +554,19 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" style="6" width="13.005" customWidth="1" bestFit="1"/>
-    <col min="2" max="2" style="6" width="13.005" customWidth="1" bestFit="1"/>
-    <col min="3" max="3" style="7" width="13.005" customWidth="1" bestFit="1"/>
-    <col min="4" max="4" style="6" width="13.005" customWidth="1" bestFit="1"/>
-    <col min="5" max="5" style="6" width="13.005" customWidth="1" bestFit="1"/>
-    <col min="6" max="6" style="6" width="13.005" customWidth="1" bestFit="1"/>
-    <col min="7" max="7" style="6" width="13.005" customWidth="1" bestFit="1"/>
-    <col min="8" max="8" style="6" width="13.005" customWidth="1" bestFit="1"/>
-    <col min="9" max="9" style="6" width="13.005" customWidth="1" bestFit="1"/>
-    <col min="10" max="10" style="6" width="13.005" customWidth="1" bestFit="1"/>
+    <col min="1" max="1" style="5" width="13.005" customWidth="1" bestFit="1"/>
+    <col min="2" max="2" style="5" width="13.005" customWidth="1" bestFit="1"/>
+    <col min="3" max="3" style="6" width="13.005" customWidth="1" bestFit="1"/>
+    <col min="4" max="4" style="5" width="13.005" customWidth="1" bestFit="1"/>
+    <col min="5" max="5" style="5" width="13.005" customWidth="1" bestFit="1"/>
+    <col min="6" max="6" style="5" width="13.005" customWidth="1" bestFit="1"/>
+    <col min="7" max="7" style="5" width="13.005" customWidth="1" bestFit="1"/>
+    <col min="8" max="8" style="5" width="13.005" customWidth="1" bestFit="1"/>
+    <col min="9" max="9" style="5" width="13.005" customWidth="1" bestFit="1"/>
+    <col min="10" max="10" style="5" width="13.005" customWidth="1" bestFit="1"/>
   </cols>
   <sheetData>
-    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="20.25">
+    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="19.5">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -605,7 +596,7 @@
         <v>8</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="19.5">
+    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="18.75">
       <c r="A2" s="3" t="s">
         <v>9</v>
       </c>
@@ -631,7 +622,7 @@
         <v>13</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="19.5">
+    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="18.75">
       <c r="A3" s="3" t="s">
         <v>14</v>
       </c>
@@ -659,7 +650,7 @@
         <v>18</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="19.5">
+    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="18.75">
       <c r="A4" s="3" t="s">
         <v>19</v>
       </c>
@@ -685,7 +676,7 @@
         <v>22</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="19.5">
+    <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="18.75">
       <c r="A5" s="3" t="s">
         <v>23</v>
       </c>
@@ -711,7 +702,7 @@
         <v>27</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="19.5">
+    <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="18.75">
       <c r="A6" s="3" t="s">
         <v>28</v>
       </c>
@@ -733,7 +724,7 @@
       <c r="I6" s="3"/>
       <c r="J6" s="3"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="19.5">
+    <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="18.75">
       <c r="A7" s="3" t="s">
         <v>30</v>
       </c>
@@ -759,7 +750,7 @@
         <v>33</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="19.5">
+    <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="18.75">
       <c r="A8" s="3" t="s">
         <v>34</v>
       </c>
@@ -781,7 +772,7 @@
       <c r="I8" s="3"/>
       <c r="J8" s="3"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="19.5">
+    <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="18.75">
       <c r="A9" s="3" t="s">
         <v>36</v>
       </c>
@@ -803,7 +794,7 @@
       <c r="I9" s="3"/>
       <c r="J9" s="3"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="10" customHeight="1" ht="19.5">
+    <row x14ac:dyDescent="0.25" r="10" customHeight="1" ht="18.75">
       <c r="A10" s="3" t="s">
         <v>38</v>
       </c>
@@ -825,7 +816,7 @@
       <c r="I10" s="3"/>
       <c r="J10" s="3"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="11" customHeight="1" ht="19.5">
+    <row x14ac:dyDescent="0.25" r="11" customHeight="1" ht="18.75">
       <c r="A11" s="3"/>
       <c r="B11" s="3"/>
       <c r="C11" s="4"/>
@@ -837,7 +828,7 @@
       <c r="I11" s="3"/>
       <c r="J11" s="3"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="12" customHeight="1" ht="19.5">
+    <row x14ac:dyDescent="0.25" r="12" customHeight="1" ht="18.75">
       <c r="A12" s="3"/>
       <c r="B12" s="3"/>
       <c r="C12" s="4"/>
@@ -849,7 +840,7 @@
       <c r="I12" s="3"/>
       <c r="J12" s="3"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="13" customHeight="1" ht="19.5">
+    <row x14ac:dyDescent="0.25" r="13" customHeight="1" ht="18.75">
       <c r="A13" s="3"/>
       <c r="B13" s="3"/>
       <c r="C13" s="4"/>
@@ -861,7 +852,7 @@
       <c r="I13" s="3"/>
       <c r="J13" s="3"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="14" customHeight="1" ht="19.5">
+    <row x14ac:dyDescent="0.25" r="14" customHeight="1" ht="18.75">
       <c r="A14" s="3"/>
       <c r="B14" s="3"/>
       <c r="C14" s="4"/>
@@ -873,7 +864,7 @@
       <c r="I14" s="3"/>
       <c r="J14" s="3"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="15" customHeight="1" ht="19.5">
+    <row x14ac:dyDescent="0.25" r="15" customHeight="1" ht="18.75">
       <c r="A15" s="3"/>
       <c r="B15" s="3"/>
       <c r="C15" s="4"/>
@@ -885,7 +876,7 @@
       <c r="I15" s="3"/>
       <c r="J15" s="3"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="16" customHeight="1" ht="19.5">
+    <row x14ac:dyDescent="0.25" r="16" customHeight="1" ht="18.75">
       <c r="A16" s="3"/>
       <c r="B16" s="3"/>
       <c r="C16" s="4"/>
@@ -897,7 +888,7 @@
       <c r="I16" s="3"/>
       <c r="J16" s="3"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="17" customHeight="1" ht="19.5">
+    <row x14ac:dyDescent="0.25" r="17" customHeight="1" ht="18.75">
       <c r="A17" s="3" t="s">
         <v>40</v>
       </c>
@@ -921,7 +912,7 @@
       <c r="I17" s="3"/>
       <c r="J17" s="3"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="18" customHeight="1" ht="19.5">
+    <row x14ac:dyDescent="0.25" r="18" customHeight="1" ht="18.75">
       <c r="A18" s="3" t="s">
         <v>43</v>
       </c>
@@ -945,14 +936,14 @@
       <c r="I18" s="3"/>
       <c r="J18" s="3"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="19" customHeight="1" ht="17.25">
+    <row x14ac:dyDescent="0.25" r="19" customHeight="1" ht="18.75">
       <c r="A19" s="3" t="s">
         <v>45</v>
       </c>
       <c r="B19" s="3" t="s">
         <v>46</v>
       </c>
-      <c r="C19" s="5">
+      <c r="C19" s="4">
         <v>13.2</v>
       </c>
       <c r="D19" s="3" t="s">
@@ -969,14 +960,14 @@
       <c r="I19" s="3"/>
       <c r="J19" s="3"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="20" customHeight="1" ht="17.25">
+    <row x14ac:dyDescent="0.25" r="20" customHeight="1" ht="18.75">
       <c r="A20" s="3" t="s">
         <v>47</v>
       </c>
       <c r="B20" s="3" t="s">
         <v>48</v>
       </c>
-      <c r="C20" s="5">
+      <c r="C20" s="4">
         <v>0.63</v>
       </c>
       <c r="D20" s="3" t="s">
@@ -993,14 +984,14 @@
       <c r="I20" s="3"/>
       <c r="J20" s="3"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="21" customHeight="1" ht="17.25">
+    <row x14ac:dyDescent="0.25" r="21" customHeight="1" ht="18.75">
       <c r="A21" s="3" t="s">
         <v>50</v>
       </c>
       <c r="B21" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="C21" s="5">
+      <c r="C21" s="4">
         <v>0.2</v>
       </c>
       <c r="D21" s="3" t="s">

</xml_diff>